<commit_message>
-Added more test  data to the correlation folder -Updated book
</commit_message>
<xml_diff>
--- a/Feasability Analysis Results/InputsAndAlgorithmsRuntimeCorrelation/TestResults_03-05-2024_gem5_400mhz_numberOfPoints_change.xlsx
+++ b/Feasability Analysis Results/InputsAndAlgorithmsRuntimeCorrelation/TestResults_03-05-2024_gem5_400mhz_numberOfPoints_change.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halel\Desktop\Project\Dev\Feasability Analysis Results\InputsAndAlgorithmsRuntimeCorrelation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B5615B4A-A07F-4E47-9AA4-0C988C6FDFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32EA0BA-14FB-4F09-AAFC-2517468B10D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestResults_03-05-2024_11-16-17" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId2"/>
+    <pivotCache cacheId="13" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="30">
   <si>
     <t>Test ID</t>
   </si>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -675,7 +675,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[TestResults_03-05-2024_gem5_400mhz_numberOfPoints_change_raw_data.xlsx]TestResults_03-05-2024_11-16-17!PivotTable1</c:name>
+    <c:name>[TestResults_03-05-2024_gem5_400mhz_numberOfPoints_change.xlsx]TestResults_03-05-2024_11-16-17!PivotTable1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1306,7 +1306,7 @@
                   <c:v>5.3323000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.9000499999999942E-2</c:v>
+                  <c:v>5.9000499999999956E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>6.0327999999999903E-2</c:v>
@@ -1363,7 +1363,7 @@
                   <c:v>7.8986000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>8.204504999999998E-2</c:v>
+                  <c:v>8.2045049999999953E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>8.36869999999999E-2</c:v>
@@ -1408,416 +1408,6 @@
           <c:tx>
             <c:strRef>
               <c:f>'TestResults_03-05-2024_11-16-17'!$AH$18:$AH$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CATCH</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'TestResults_03-05-2024_11-16-17'!$AF$20:$AF$80</c:f>
-              <c:strCache>
-                <c:ptCount val="60"/>
-                <c:pt idx="0">
-                  <c:v>1441</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1456</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1501</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1531</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1546</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1561</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1591</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2881</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2896</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2926</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3061</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3106</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3121</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3181</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4321</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4351</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4396</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4516</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4591</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4651</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4681</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4771</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5761</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5806</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5866</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>6016</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>6121</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>6211</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>6241</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>6361</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>7216</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>7246</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>7321</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7336</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>7516</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>7531</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>7651</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7756</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>7801</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>7951</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>8656</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>8701</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>8791</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>8806</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>9031</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>9181</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>9316</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>9361</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>9556</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>10096</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>10156</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>10261</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>10276</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>10531</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>10546</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>10711</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>10861</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>10921</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>11146</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'TestResults_03-05-2024_11-16-17'!$AH$20:$AH$80</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
-                <c:pt idx="0">
-                  <c:v>0.31321195238095167</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.31673099999999899</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.3248065</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.331284999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.337060999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.33879500000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.341884999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.64683004999999938</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.60909800000000003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.62660749999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.64281699999999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.66895199999999899</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.67414099999999899</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.67808599999999897</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.68691199999999897</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.85649684999999953</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.97215799999999897</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.9613079999999995</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.98883349999999903</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.99113700000000005</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.94730000000000003</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.99001499999999898</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.01002199999999</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.0737390999999945</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.1400490000000001</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.1420184999999901</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.1593364999999949</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.173532</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.16318399999999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.1813940000000001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.1916340000000001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.322577749999996</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1.34714299999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.356719</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.4334880000000001</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1.391348</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1.4023030000000001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.4269099999999899</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.39319499999999</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1.45027799999999</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.4869619999999899</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1.6042302499999945</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1.61271399999999</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.7014260000000001</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.61763699999999</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>1.6684220000000001</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1.6894340000000001</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1.6604859999999899</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1.7050000000000001</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>1.84589</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1.8506113499999941</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>1.8237080000000001</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>1.8715250000000001</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1.9563539999999899</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>1.919502</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>1.9149400000000001</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>1.94876899999999</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>1.926188</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1.9679770000000001</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>2.1030690000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-1D3E-4A82-BBA0-AC7B21B13178}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'TestResults_03-05-2024_11-16-17'!$AI$18:$AI$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2028,7 +1618,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TestResults_03-05-2024_11-16-17'!$AI$20:$AI$80</c:f>
+              <c:f>'TestResults_03-05-2024_11-16-17'!$AH$20:$AH$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -2126,7 +1716,7 @@
                   <c:v>0.19501199999999899</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.14402109999999949</c:v>
+                  <c:v>0.14402109999999943</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0.19115599999999899</c:v>
@@ -2218,7 +1808,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-1D3E-4A82-BBA0-AC7B21B13178}"/>
+              <c16:uniqueId val="{00000007-1D3E-4A82-BBA0-AC7B21B13178}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2455,10 +2045,10 @@
       <xdr:rowOff>100010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>67</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2487,7 +2077,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Hallel Weil" refreshedDate="45415.951363888889" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="609">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Hallel Weil" refreshedDate="45415.951363888889" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="609" xr:uid="{00000000-000A-0000-FFFF-FFFF04000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:W610" sheet="TestResults_03-05-2024_11-16-17"/>
   </cacheSource>
@@ -17866,15 +17456,15 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
-  <location ref="AF18:AJ80" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+  <location ref="AF18:AI80" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="23">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
       <items count="4">
         <item x="0"/>
-        <item x="2"/>
+        <item h="1" x="2"/>
         <item x="1"/>
         <item t="default"/>
       </items>
@@ -18155,12 +17745,9 @@
   <colFields count="1">
     <field x="2"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="3">
     <i>
       <x/>
-    </i>
-    <i>
-      <x v="1"/>
     </i>
     <i>
       <x v="2"/>
@@ -18590,11 +18177,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ610"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AI610"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BC12" sqref="BC12"/>
+    <sheetView tabSelected="1" topLeftCell="AM13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BU42" sqref="BU42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19740,7 +19327,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -19811,7 +19398,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -19888,7 +19475,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -19965,16 +19552,13 @@
         <v>23</v>
       </c>
       <c r="AH19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AI19" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -20051,16 +19635,13 @@
         <v>1.2813952380952343E-2</v>
       </c>
       <c r="AH20" s="3">
-        <v>0.31321195238095167</v>
+        <v>0.12681261904761876</v>
       </c>
       <c r="AI20" s="3">
-        <v>0.12681261904761876</v>
-      </c>
-      <c r="AJ20" s="3">
-        <v>0.1509461746031743</v>
+        <v>6.9813285714285536E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -20137,16 +19718,13 @@
         <v>1.38094999999999E-2</v>
       </c>
       <c r="AH21" s="3">
-        <v>0.31673099999999899</v>
+        <v>0.19622499999999898</v>
       </c>
       <c r="AI21" s="3">
-        <v>0.19622499999999898</v>
-      </c>
-      <c r="AJ21" s="3">
-        <v>0.17558849999999929</v>
+        <v>0.10501724999999945</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -20223,16 +19801,13 @@
         <v>1.4199999999999951E-2</v>
       </c>
       <c r="AH22" s="3">
-        <v>0.3248065</v>
+        <v>0.19929649999999949</v>
       </c>
       <c r="AI22" s="3">
-        <v>0.19929649999999949</v>
-      </c>
-      <c r="AJ22" s="3">
-        <v>0.17943433333333317</v>
+        <v>0.10674824999999973</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -20309,16 +19884,13 @@
         <v>1.4474000000000001E-2</v>
       </c>
       <c r="AH23" s="3">
-        <v>0.331284999999999</v>
+        <v>0.201565999999999</v>
       </c>
       <c r="AI23" s="3">
-        <v>0.201565999999999</v>
-      </c>
-      <c r="AJ23" s="3">
-        <v>0.18244166666666597</v>
+        <v>0.10801999999999951</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -20395,16 +19967,13 @@
         <v>1.4352E-2</v>
       </c>
       <c r="AH24" s="3">
-        <v>0.337060999999999</v>
+        <v>0.15035000000000001</v>
       </c>
       <c r="AI24" s="3">
-        <v>0.15035000000000001</v>
-      </c>
-      <c r="AJ24" s="3">
-        <v>0.16725433333333298</v>
+        <v>8.2351000000000008E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -20481,16 +20050,13 @@
         <v>1.4791999999999901E-2</v>
       </c>
       <c r="AH25" s="3">
-        <v>0.33879500000000001</v>
+        <v>0.20774500000000001</v>
       </c>
       <c r="AI25" s="3">
-        <v>0.20774500000000001</v>
-      </c>
-      <c r="AJ25" s="3">
-        <v>0.18711066666666665</v>
+        <v>0.11126849999999995</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -20567,16 +20133,13 @@
         <v>1.4996999999999899E-2</v>
       </c>
       <c r="AH26" s="3">
-        <v>0.341884999999999</v>
+        <v>0.207872</v>
       </c>
       <c r="AI26" s="3">
-        <v>0.207872</v>
-      </c>
-      <c r="AJ26" s="3">
-        <v>0.18825133333333297</v>
+        <v>0.11143449999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -20653,16 +20216,13 @@
         <v>2.4303199999999931E-2</v>
       </c>
       <c r="AH27" s="3">
-        <v>0.64683004999999938</v>
+        <v>0.12085824999999961</v>
       </c>
       <c r="AI27" s="3">
-        <v>0.12085824999999961</v>
-      </c>
-      <c r="AJ27" s="3">
-        <v>0.26399716666666628</v>
+        <v>7.2580724999999763E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -20739,16 +20299,13 @@
         <v>2.5388000000000001E-2</v>
       </c>
       <c r="AH28" s="3">
-        <v>0.60909800000000003</v>
+        <v>0.18498500000000001</v>
       </c>
       <c r="AI28" s="3">
-        <v>0.18498500000000001</v>
-      </c>
-      <c r="AJ28" s="3">
-        <v>0.27315700000000004</v>
+        <v>0.1051865</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -20825,16 +20382,13 @@
         <v>2.5642999999999902E-2</v>
       </c>
       <c r="AH29" s="3">
-        <v>0.62660749999999998</v>
+        <v>0.1884689999999995</v>
       </c>
       <c r="AI29" s="3">
-        <v>0.1884689999999995</v>
-      </c>
-      <c r="AJ29" s="3">
-        <v>0.28023983333333313</v>
+        <v>0.10705599999999971</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -20911,16 +20465,13 @@
         <v>2.624649999999995E-2</v>
       </c>
       <c r="AH30" s="3">
-        <v>0.64281699999999997</v>
+        <v>0.18825799999999898</v>
       </c>
       <c r="AI30" s="3">
-        <v>0.18825799999999898</v>
-      </c>
-      <c r="AJ30" s="3">
-        <v>0.285773833333333</v>
+        <v>0.10725224999999947</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -20997,16 +20548,13 @@
         <v>2.6780000000000002E-2</v>
       </c>
       <c r="AH31" s="3">
-        <v>0.66895199999999899</v>
+        <v>0.18565100000000001</v>
       </c>
       <c r="AI31" s="3">
-        <v>0.18565100000000001</v>
-      </c>
-      <c r="AJ31" s="3">
-        <v>0.29379433333333299</v>
+        <v>0.1062155</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -21083,16 +20631,13 @@
         <v>2.6942000000000001E-2</v>
       </c>
       <c r="AH32" s="3">
-        <v>0.67414099999999899</v>
+        <v>0.166767999999999</v>
       </c>
       <c r="AI32" s="3">
-        <v>0.166767999999999</v>
-      </c>
-      <c r="AJ32" s="3">
-        <v>0.289283666666666</v>
+        <v>9.6854999999999497E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -21169,16 +20714,13 @@
         <v>2.7380999999999898E-2</v>
       </c>
       <c r="AH33" s="3">
-        <v>0.67808599999999897</v>
+        <v>0.18836600000000001</v>
       </c>
       <c r="AI33" s="3">
-        <v>0.18836600000000001</v>
-      </c>
-      <c r="AJ33" s="3">
-        <v>0.29794433333333298</v>
+        <v>0.10787349999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -21255,16 +20797,13 @@
         <v>2.7785000000000001E-2</v>
       </c>
       <c r="AH34" s="3">
-        <v>0.68691199999999897</v>
+        <v>0.195878999999999</v>
       </c>
       <c r="AI34" s="3">
-        <v>0.195878999999999</v>
-      </c>
-      <c r="AJ34" s="3">
-        <v>0.30352533333333265</v>
+        <v>0.1118319999999995</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -21341,16 +20880,13 @@
         <v>3.5827799999999951E-2</v>
       </c>
       <c r="AH35" s="3">
-        <v>0.85649684999999953</v>
+        <v>0.12588814999999948</v>
       </c>
       <c r="AI35" s="3">
-        <v>0.12588814999999948</v>
-      </c>
-      <c r="AJ35" s="3">
-        <v>0.33940426666666629</v>
+        <v>8.0857974999999721E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -21427,16 +20963,13 @@
         <v>3.7086000000000001E-2</v>
       </c>
       <c r="AH36" s="3">
-        <v>0.97215799999999897</v>
+        <v>0.18451500000000001</v>
       </c>
       <c r="AI36" s="3">
-        <v>0.18451500000000001</v>
-      </c>
-      <c r="AJ36" s="3">
-        <v>0.39791966666666628</v>
+        <v>0.11080050000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -21513,16 +21046,13 @@
         <v>3.7455999999999948E-2</v>
       </c>
       <c r="AH37" s="3">
-        <v>0.9613079999999995</v>
+        <v>0.183202</v>
       </c>
       <c r="AI37" s="3">
-        <v>0.183202</v>
-      </c>
-      <c r="AJ37" s="3">
-        <v>0.39398866666666649</v>
+        <v>0.11032899999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -21599,16 +21129,13 @@
         <v>3.8433000000000002E-2</v>
       </c>
       <c r="AH38" s="3">
-        <v>0.98883349999999903</v>
+        <v>0.18480400000000002</v>
       </c>
       <c r="AI38" s="3">
-        <v>0.18480400000000002</v>
-      </c>
-      <c r="AJ38" s="3">
-        <v>0.40402349999999965</v>
+        <v>0.11161850000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -21685,16 +21212,13 @@
         <v>3.9075999999999902E-2</v>
       </c>
       <c r="AH39" s="3">
-        <v>0.99113700000000005</v>
+        <v>0.188334</v>
       </c>
       <c r="AI39" s="3">
-        <v>0.188334</v>
-      </c>
-      <c r="AJ39" s="3">
-        <v>0.40618233333333337</v>
+        <v>0.11370499999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -21771,16 +21295,13 @@
         <v>3.9377000000000002E-2</v>
       </c>
       <c r="AH40" s="3">
-        <v>0.94730000000000003</v>
+        <v>0.178372</v>
       </c>
       <c r="AI40" s="3">
-        <v>0.178372</v>
-      </c>
-      <c r="AJ40" s="3">
-        <v>0.38834966666666665</v>
+        <v>0.1088745</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -21857,16 +21378,13 @@
         <v>3.99549999999999E-2</v>
       </c>
       <c r="AH41" s="3">
-        <v>0.99001499999999898</v>
+        <v>0.19339999999999899</v>
       </c>
       <c r="AI41" s="3">
-        <v>0.19339999999999899</v>
-      </c>
-      <c r="AJ41" s="3">
-        <v>0.40778999999999926</v>
+        <v>0.11667749999999945</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -21943,16 +21461,13 @@
         <v>4.0556000000000002E-2</v>
       </c>
       <c r="AH42" s="3">
-        <v>1.01002199999999</v>
+        <v>0.19233900000000001</v>
       </c>
       <c r="AI42" s="3">
-        <v>0.19233900000000001</v>
-      </c>
-      <c r="AJ42" s="3">
-        <v>0.41430566666666335</v>
+        <v>0.11644750000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -22029,16 +21544,13 @@
         <v>4.735284999999996E-2</v>
       </c>
       <c r="AH43" s="3">
-        <v>1.0737390999999945</v>
+        <v>0.1340725999999996</v>
       </c>
       <c r="AI43" s="3">
-        <v>0.1340725999999996</v>
-      </c>
-      <c r="AJ43" s="3">
-        <v>0.41838818333333128</v>
+        <v>9.0712724999999786E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -22115,16 +21627,13 @@
         <v>4.87519999999999E-2</v>
       </c>
       <c r="AH44" s="3">
-        <v>1.1400490000000001</v>
+        <v>0.187389</v>
       </c>
       <c r="AI44" s="3">
-        <v>0.187389</v>
-      </c>
-      <c r="AJ44" s="3">
-        <v>0.45873000000000003</v>
+        <v>0.11807049999999995</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -22201,16 +21710,13 @@
         <v>4.9262999999999904E-2</v>
       </c>
       <c r="AH45" s="3">
-        <v>1.1420184999999901</v>
+        <v>0.18645300000000001</v>
       </c>
       <c r="AI45" s="3">
-        <v>0.18645300000000001</v>
-      </c>
-      <c r="AJ45" s="3">
-        <v>0.45924483333332994</v>
+        <v>0.11785799999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -22287,16 +21793,13 @@
         <v>5.0481999999999999E-2</v>
       </c>
       <c r="AH46" s="3">
-        <v>1.1593364999999949</v>
+        <v>0.19270599999999949</v>
       </c>
       <c r="AI46" s="3">
-        <v>0.19270599999999949</v>
-      </c>
-      <c r="AJ46" s="3">
-        <v>0.46750816666666478</v>
+        <v>0.12159399999999974</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -22373,16 +21876,13 @@
         <v>5.1361999999999901E-2</v>
       </c>
       <c r="AH47" s="3">
-        <v>1.173532</v>
+        <v>0.195599999999999</v>
       </c>
       <c r="AI47" s="3">
-        <v>0.195599999999999</v>
-      </c>
-      <c r="AJ47" s="3">
-        <v>0.47349799999999959</v>
+        <v>0.12348099999999945</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -22459,16 +21959,13 @@
         <v>5.19369999999999E-2</v>
       </c>
       <c r="AH48" s="3">
-        <v>1.16318399999999</v>
+        <v>0.185477</v>
       </c>
       <c r="AI48" s="3">
-        <v>0.185477</v>
-      </c>
-      <c r="AJ48" s="3">
-        <v>0.46686599999999662</v>
+        <v>0.11870699999999995</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -22545,16 +22042,13 @@
         <v>5.2527999999999901E-2</v>
       </c>
       <c r="AH49" s="3">
-        <v>1.1813940000000001</v>
+        <v>0.19522</v>
       </c>
       <c r="AI49" s="3">
-        <v>0.19522</v>
-      </c>
-      <c r="AJ49" s="3">
-        <v>0.47638066666666662</v>
+        <v>0.12387399999999996</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -22631,16 +22125,13 @@
         <v>5.3323000000000002E-2</v>
       </c>
       <c r="AH50" s="3">
-        <v>1.1916340000000001</v>
+        <v>0.19501199999999899</v>
       </c>
       <c r="AI50" s="3">
-        <v>0.19501199999999899</v>
-      </c>
-      <c r="AJ50" s="3">
-        <v>0.47998966666666637</v>
+        <v>0.1241674999999995</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -22714,19 +22205,16 @@
         <v>7216</v>
       </c>
       <c r="AG51" s="3">
-        <v>5.9000499999999942E-2</v>
+        <v>5.9000499999999956E-2</v>
       </c>
       <c r="AH51" s="3">
-        <v>1.322577749999996</v>
+        <v>0.14402109999999943</v>
       </c>
       <c r="AI51" s="3">
-        <v>0.14402109999999949</v>
-      </c>
-      <c r="AJ51" s="3">
-        <v>0.50853311666666523</v>
+        <v>0.10151079999999971</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -22803,16 +22291,13 @@
         <v>6.0327999999999903E-2</v>
       </c>
       <c r="AH52" s="3">
-        <v>1.34714299999999</v>
+        <v>0.19115599999999899</v>
       </c>
       <c r="AI52" s="3">
-        <v>0.19115599999999899</v>
-      </c>
-      <c r="AJ52" s="3">
-        <v>0.53287566666666297</v>
+        <v>0.12574199999999944</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -22889,16 +22374,13 @@
         <v>6.0930999999999902E-2</v>
       </c>
       <c r="AH53" s="3">
-        <v>1.356719</v>
+        <v>0.192771999999999</v>
       </c>
       <c r="AI53" s="3">
-        <v>0.192771999999999</v>
-      </c>
-      <c r="AJ53" s="3">
-        <v>0.53680733333333297</v>
+        <v>0.12685149999999945</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -22975,16 +22457,13 @@
         <v>6.1059000000000002E-2</v>
       </c>
       <c r="AH54" s="3">
-        <v>1.4334880000000001</v>
+        <v>0.194831</v>
       </c>
       <c r="AI54" s="3">
-        <v>0.194831</v>
-      </c>
-      <c r="AJ54" s="3">
-        <v>0.56312600000000002</v>
+        <v>0.127945</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -23061,16 +22540,13 @@
         <v>6.2539999999999901E-2</v>
       </c>
       <c r="AH55" s="3">
-        <v>1.391348</v>
+        <v>0.195828</v>
       </c>
       <c r="AI55" s="3">
-        <v>0.195828</v>
-      </c>
-      <c r="AJ55" s="3">
-        <v>0.54990533333333325</v>
+        <v>0.12918399999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -23147,16 +22623,13 @@
         <v>6.2656000000000003E-2</v>
       </c>
       <c r="AH56" s="3">
-        <v>1.4023030000000001</v>
+        <v>0.195099999999999</v>
       </c>
       <c r="AI56" s="3">
-        <v>0.195099999999999</v>
-      </c>
-      <c r="AJ56" s="3">
-        <v>0.55335299999999965</v>
+        <v>0.12887799999999949</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -23233,16 +22706,13 @@
         <v>6.3649999999999901E-2</v>
       </c>
       <c r="AH57" s="3">
-        <v>1.4269099999999899</v>
+        <v>0.19853899999999899</v>
       </c>
       <c r="AI57" s="3">
-        <v>0.19853899999999899</v>
-      </c>
-      <c r="AJ57" s="3">
-        <v>0.56303299999999623</v>
+        <v>0.13109449999999945</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -23319,16 +22789,13 @@
         <v>6.4378000000000005E-2</v>
       </c>
       <c r="AH58" s="3">
-        <v>1.39319499999999</v>
+        <v>0.195493</v>
       </c>
       <c r="AI58" s="3">
-        <v>0.195493</v>
-      </c>
-      <c r="AJ58" s="3">
-        <v>0.55102199999999668</v>
+        <v>0.12993550000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -23405,16 +22872,13 @@
         <v>6.5082000000000001E-2</v>
       </c>
       <c r="AH59" s="3">
-        <v>1.45027799999999</v>
+        <v>0.205597</v>
       </c>
       <c r="AI59" s="3">
-        <v>0.205597</v>
-      </c>
-      <c r="AJ59" s="3">
-        <v>0.57365233333332999</v>
+        <v>0.1353395</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -23491,16 +22955,13 @@
         <v>6.6082000000000002E-2</v>
       </c>
       <c r="AH60" s="3">
-        <v>1.4869619999999899</v>
+        <v>0.20532300000000001</v>
       </c>
       <c r="AI60" s="3">
-        <v>0.20532300000000001</v>
-      </c>
-      <c r="AJ60" s="3">
-        <v>0.58612233333332997</v>
+        <v>0.1357025</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -23577,16 +23038,13 @@
         <v>7.0522649999999965E-2</v>
       </c>
       <c r="AH61" s="3">
-        <v>1.6042302499999945</v>
+        <v>0.15373214999999929</v>
       </c>
       <c r="AI61" s="3">
-        <v>0.15373214999999929</v>
-      </c>
-      <c r="AJ61" s="3">
-        <v>0.60949501666666461</v>
+        <v>0.11212739999999961</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -23663,16 +23121,13 @@
         <v>7.2009000000000004E-2</v>
       </c>
       <c r="AH62" s="3">
-        <v>1.61271399999999</v>
+        <v>0.20233100000000001</v>
       </c>
       <c r="AI62" s="3">
-        <v>0.20233100000000001</v>
-      </c>
-      <c r="AJ62" s="3">
-        <v>0.62901799999999664</v>
+        <v>0.13717000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -23749,16 +23204,13 @@
         <v>7.2746000000000005E-2</v>
       </c>
       <c r="AH63" s="3">
-        <v>1.7014260000000001</v>
+        <v>0.202427999999999</v>
       </c>
       <c r="AI63" s="3">
-        <v>0.202427999999999</v>
-      </c>
-      <c r="AJ63" s="3">
-        <v>0.65886666666666638</v>
+        <v>0.13758699999999952</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -23835,16 +23287,13 @@
         <v>7.2847999999999899E-2</v>
       </c>
       <c r="AH64" s="3">
-        <v>1.61763699999999</v>
+        <v>0.20196600000000001</v>
       </c>
       <c r="AI64" s="3">
-        <v>0.20196600000000001</v>
-      </c>
-      <c r="AJ64" s="3">
-        <v>0.63081699999999663</v>
+        <v>0.13740699999999995</v>
       </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -23921,16 +23370,13 @@
         <v>7.4650500000000009E-2</v>
       </c>
       <c r="AH65" s="3">
-        <v>1.6684220000000001</v>
+        <v>0.2006289999999995</v>
       </c>
       <c r="AI65" s="3">
-        <v>0.2006289999999995</v>
-      </c>
-      <c r="AJ65" s="3">
-        <v>0.64790049999999988</v>
+        <v>0.13763974999999976</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -24007,16 +23453,13 @@
         <v>7.5937000000000004E-2</v>
       </c>
       <c r="AH66" s="3">
-        <v>1.6894340000000001</v>
+        <v>0.20907500000000001</v>
       </c>
       <c r="AI66" s="3">
-        <v>0.20907500000000001</v>
-      </c>
-      <c r="AJ66" s="3">
-        <v>0.6581486666666666</v>
+        <v>0.14250600000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -24093,16 +23536,13 @@
         <v>7.6926999999999898E-2</v>
       </c>
       <c r="AH67" s="3">
-        <v>1.6604859999999899</v>
+        <v>0.20849699999999899</v>
       </c>
       <c r="AI67" s="3">
-        <v>0.20849699999999899</v>
-      </c>
-      <c r="AJ67" s="3">
-        <v>0.64863666666666298</v>
+        <v>0.14271199999999945</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -24179,16 +23619,13 @@
         <v>7.7671000000000004E-2</v>
       </c>
       <c r="AH68" s="3">
-        <v>1.7050000000000001</v>
+        <v>0.21121400000000001</v>
       </c>
       <c r="AI68" s="3">
-        <v>0.21121400000000001</v>
-      </c>
-      <c r="AJ68" s="3">
-        <v>0.66462833333333338</v>
+        <v>0.1444425</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -24265,16 +23702,13 @@
         <v>7.8986000000000001E-2</v>
       </c>
       <c r="AH69" s="3">
-        <v>1.84589</v>
+        <v>0.21248400000000001</v>
       </c>
       <c r="AI69" s="3">
-        <v>0.21248400000000001</v>
-      </c>
-      <c r="AJ69" s="3">
-        <v>0.71245333333333338</v>
+        <v>0.145735</v>
       </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -24348,19 +23782,16 @@
         <v>10096</v>
       </c>
       <c r="AG70" s="3">
-        <v>8.204504999999998E-2</v>
+        <v>8.2045049999999953E-2</v>
       </c>
       <c r="AH70" s="3">
-        <v>1.8506113499999941</v>
+        <v>0.16452294999999945</v>
       </c>
       <c r="AI70" s="3">
-        <v>0.16452294999999945</v>
-      </c>
-      <c r="AJ70" s="3">
-        <v>0.69905978333333108</v>
+        <v>0.12328399999999969</v>
       </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -24437,16 +23868,13 @@
         <v>8.36869999999999E-2</v>
       </c>
       <c r="AH71" s="3">
-        <v>1.8237080000000001</v>
+        <v>0.21087</v>
       </c>
       <c r="AI71" s="3">
-        <v>0.21087</v>
-      </c>
-      <c r="AJ71" s="3">
-        <v>0.70608833333333332</v>
+        <v>0.14727849999999995</v>
       </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -24523,16 +23951,13 @@
         <v>8.4545999999999899E-2</v>
       </c>
       <c r="AH72" s="3">
-        <v>1.8715250000000001</v>
+        <v>0.21365400000000001</v>
       </c>
       <c r="AI72" s="3">
-        <v>0.21365400000000001</v>
-      </c>
-      <c r="AJ72" s="3">
-        <v>0.72324166666666667</v>
+        <v>0.14909999999999995</v>
       </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -24609,16 +24034,13 @@
         <v>8.4665000000000004E-2</v>
       </c>
       <c r="AH73" s="3">
-        <v>1.9563539999999899</v>
+        <v>0.213174</v>
       </c>
       <c r="AI73" s="3">
-        <v>0.213174</v>
-      </c>
-      <c r="AJ73" s="3">
-        <v>0.75139766666666341</v>
+        <v>0.14891950000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -24695,16 +24117,13 @@
         <v>8.6751999999999899E-2</v>
       </c>
       <c r="AH74" s="3">
-        <v>1.919502</v>
+        <v>0.21302699999999899</v>
       </c>
       <c r="AI74" s="3">
-        <v>0.21302699999999899</v>
-      </c>
-      <c r="AJ74" s="3">
-        <v>0.73976033333333291</v>
+        <v>0.14988949999999945</v>
       </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -24781,16 +24200,13 @@
         <v>8.6866999999999903E-2</v>
       </c>
       <c r="AH75" s="3">
-        <v>1.9149400000000001</v>
+        <v>0.22129299999999899</v>
       </c>
       <c r="AI75" s="3">
-        <v>0.22129299999999899</v>
-      </c>
-      <c r="AJ75" s="3">
-        <v>0.74103333333333288</v>
+        <v>0.15407999999999944</v>
       </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -24867,16 +24283,13 @@
         <v>8.8174000000000002E-2</v>
       </c>
       <c r="AH76" s="3">
-        <v>1.94876899999999</v>
+        <v>0.21560199999999899</v>
       </c>
       <c r="AI76" s="3">
-        <v>0.21560199999999899</v>
-      </c>
-      <c r="AJ76" s="3">
-        <v>0.75084833333332979</v>
+        <v>0.1518879999999995</v>
       </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -24953,16 +24366,13 @@
         <v>8.9358000000000007E-2</v>
       </c>
       <c r="AH77" s="3">
-        <v>1.926188</v>
+        <v>0.21287900000000001</v>
       </c>
       <c r="AI77" s="3">
-        <v>0.21287900000000001</v>
-      </c>
-      <c r="AJ77" s="3">
-        <v>0.7428083333333334</v>
+        <v>0.15111850000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -25039,16 +24449,13 @@
         <v>9.0246999999999897E-2</v>
       </c>
       <c r="AH78" s="3">
-        <v>1.9679770000000001</v>
+        <v>0.225328</v>
       </c>
       <c r="AI78" s="3">
-        <v>0.225328</v>
-      </c>
-      <c r="AJ78" s="3">
-        <v>0.76118400000000008</v>
+        <v>0.15778749999999994</v>
       </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -25125,16 +24532,13 @@
         <v>9.1739000000000001E-2</v>
       </c>
       <c r="AH79" s="3">
-        <v>2.1030690000000001</v>
+        <v>0.228792999999999</v>
       </c>
       <c r="AI79" s="3">
-        <v>0.228792999999999</v>
-      </c>
-      <c r="AJ79" s="3">
-        <v>0.80786699999999978</v>
+        <v>0.16026599999999949</v>
       </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -25211,13 +24615,10 @@
         <v>4.8459157635467952E-2</v>
       </c>
       <c r="AH80" s="3">
-        <v>1.1167907586206864</v>
+        <v>0.15629136945812766</v>
       </c>
       <c r="AI80" s="3">
-        <v>0.15629136945812766</v>
-      </c>
-      <c r="AJ80" s="3">
-        <v>0.44051376190476083</v>
+        <v>0.10237526354679782</v>
       </c>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>